<commit_message>
Add FNO reversal scanners with hourly scheduling
- Created Long_Reversal_Daily_FNO.py and Short_Reversal_Daily_FNO.py scanners
- Scanners read from FNO_Liquid.xlsx and output to Daily/FNO/Long and Daily/FNO/Short
- Created plist files for both scanners to run hourly at :19 during market hours
- Updated job_manager_dashboard.py to include FNO scanners
- Updated documentation in DASHBOARD_JOBS_UPDATE.md
- Both scanners implement Al Brooks reversal pattern detection for F&O stocks

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Daily/Plan/Consolidated_Plan_Latest.xlsx
+++ b/Daily/Plan/Consolidated_Plan_Latest.xlsx
@@ -481,14 +481,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>THERMAX</t>
+          <t>BAJAJ-AUTO</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>3885.9</v>
+        <v>9113.405025202483</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>9.302325581395349</v>
       </c>
     </row>
     <row r="3">
@@ -497,14 +497,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TIMETECHNO</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>472.3</v>
+        <v>467.5684548757732</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>4.347826086956522</v>
+        <v>9.302325581395349</v>
       </c>
     </row>
     <row r="4">
@@ -513,14 +513,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HDFCAMC</t>
+          <t>PVRINOX</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>5510</v>
+        <v>1117.750226124427</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>4.347826086956522</v>
+        <v>6.976744186046512</v>
       </c>
     </row>
     <row r="5">
@@ -529,14 +529,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SONACOMS</t>
+          <t>LTF</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>486</v>
+        <v>224.0787602742681</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>4.347826086956522</v>
+        <v>6.976744186046512</v>
       </c>
     </row>
     <row r="6">
@@ -545,14 +545,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PATANJALI</t>
+          <t>PIIND</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>1909.3</v>
+        <v>4595.026806698306</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>4.347826086956522</v>
+        <v>2.325581395348837</v>
       </c>
     </row>
     <row r="7">
@@ -561,14 +561,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CRAFTSMAN</t>
+          <t>MASTEK</t>
         </is>
       </c>
       <c r="C7" s="3" t="n">
-        <v>6490.5</v>
+        <v>2998.999843288399</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>2.325581395348837</v>
       </c>
     </row>
     <row r="8">
@@ -577,14 +577,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SHYAMMETL</t>
+          <t>SCHAEFFLER</t>
         </is>
       </c>
       <c r="C8" s="3" t="n">
-        <v>919.8</v>
+        <v>4747.486630466043</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>2.325581395348837</v>
       </c>
     </row>
     <row r="9">
@@ -593,14 +593,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>OLECTRA</t>
+          <t>UPL</t>
         </is>
       </c>
       <c r="C9" s="3" t="n">
-        <v>1275.3</v>
+        <v>746.5463222727701</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>6.976744186046512</v>
       </c>
     </row>
     <row r="10">
@@ -609,14 +609,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CHALET</t>
+          <t>CRAFTSMAN</t>
         </is>
       </c>
       <c r="C10" s="3" t="n">
-        <v>922.25</v>
+        <v>7111.741741431812</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>2.325581395348837</v>
       </c>
     </row>
     <row r="11">
@@ -625,14 +625,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>HEG</t>
+          <t>ASHAPURMIN</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>550.45</v>
+        <v>622.7105881821097</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>4.651162790697675</v>
       </c>
     </row>
     <row r="12">
@@ -641,14 +641,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>NUVAMA</t>
+          <t>CHEMPLASTS</t>
         </is>
       </c>
       <c r="C12" s="3" t="n">
-        <v>7818.5</v>
+        <v>479.8745961253245</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>6.976744186046512</v>
       </c>
     </row>
     <row r="13">
@@ -657,14 +657,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CHEMPLASTS</t>
+          <t>METROBRAND</t>
         </is>
       </c>
       <c r="C13" s="3" t="n">
-        <v>443.45</v>
+        <v>1300.862736668633</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>2.898550724637681</v>
+        <v>2.325581395348837</v>
       </c>
     </row>
     <row r="14">
@@ -673,14 +673,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>NLCINDIA</t>
+          <t>SUNTV</t>
         </is>
       </c>
       <c r="C14" s="3" t="n">
-        <v>239.18</v>
+        <v>634.4313398645224</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>2.325581395348837</v>
       </c>
     </row>
     <row r="15">
@@ -689,14 +689,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BANKBARODA</t>
+          <t>POONAWALLA</t>
         </is>
       </c>
       <c r="C15" s="3" t="n">
-        <v>246.52</v>
+        <v>490.3154832072964</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>2.325581395348837</v>
       </c>
     </row>
     <row r="16">
@@ -705,14 +705,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>THOMASCOOK</t>
+          <t>TATAINVEST</t>
         </is>
       </c>
       <c r="C16" s="3" t="n">
-        <v>177.69</v>
+        <v>7184.423831922282</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>4.347826086956522</v>
+        <v>4.651162790697675</v>
       </c>
     </row>
     <row r="17">
@@ -721,14 +721,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CANBK</t>
+          <t>TIMKEN</t>
         </is>
       </c>
       <c r="C17" s="3" t="n">
-        <v>115.53</v>
+        <v>3561.631160176454</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>5.797101449275362</v>
+        <v>6.976744186046512</v>
       </c>
     </row>
     <row r="18">
@@ -737,14 +737,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>FORTIS</t>
+          <t>PRAKASH</t>
         </is>
       </c>
       <c r="C18" s="3" t="n">
-        <v>810.25</v>
+        <v>185.7201128938527</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>4.347826086956522</v>
+        <v>6.976744186046512</v>
       </c>
     </row>
     <row r="19">
@@ -753,14 +753,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CERA</t>
+          <t>TATASTEEL</t>
         </is>
       </c>
       <c r="C19" s="3" t="n">
-        <v>7052.5</v>
+        <v>168.7678033002403</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>4.347826086956522</v>
+        <v>4.651162790697675</v>
       </c>
     </row>
     <row r="20">
@@ -769,14 +769,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PENIND</t>
+          <t>FLUOROCHEM</t>
         </is>
       </c>
       <c r="C20" s="3" t="n">
-        <v>247.55</v>
+        <v>3653.500678453571</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>4.347826086956522</v>
+        <v>4.651162790697675</v>
       </c>
     </row>
     <row r="21">
@@ -785,14 +785,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RRKABEL</t>
+          <t>VBL</t>
         </is>
       </c>
       <c r="C21" s="3" t="n">
-        <v>1461.8</v>
+        <v>499.5081586398466</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>4.347826086956522</v>
+        <v>4.651162790697675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add FNO Liquid reversal scanners with hourly schedule
- Created Long_Reversal_Daily_FNO_Liquid.py and Short_Reversal_Daily_FNO_Liquid.py
- Scanners target FNO_Liquid.xlsx stocks specifically
- Created run_fno_liquid_reversal_scanners.py to run both scanners
- Created plist to run every hour at :19 (9:19-15:19 Mon-Fri)
- Added job to job manager dashboard
- Output goes to FNO/Long/Liquid and FNO/Short/Liquid directories
</commit_message>
<xml_diff>
--- a/Daily/Plan/Consolidated_Plan_Latest.xlsx
+++ b/Daily/Plan/Consolidated_Plan_Latest.xlsx
@@ -481,14 +481,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BAJAJ-AUTO</t>
+          <t>SHREECEM</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>9113.405025202483</v>
+        <v>34500.93347606339</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>9.302325581395349</v>
+        <v>8.888888888888889</v>
       </c>
     </row>
     <row r="3">
@@ -497,14 +497,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>CENTENKA</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>467.5684548757732</v>
+        <v>582.4419439421799</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>9.302325581395349</v>
+        <v>4.444444444444445</v>
       </c>
     </row>
     <row r="4">
@@ -513,14 +513,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PVRINOX</t>
+          <t>UPL</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>1117.750226124427</v>
+        <v>784.0190380412599</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>6.976744186046512</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="5">
@@ -529,14 +529,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LTF</t>
+          <t>PAYTM</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>224.0787602742681</v>
+        <v>1114.958294817461</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>6.976744186046512</v>
+        <v>8.888888888888889</v>
       </c>
     </row>
     <row r="6">
@@ -545,14 +545,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PIIND</t>
+          <t>SHK</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>4595.026806698306</v>
+        <v>273.9244346664965</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>2.325581395348837</v>
+        <v>8.888888888888889</v>
       </c>
     </row>
     <row r="7">
@@ -561,14 +561,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MASTEK</t>
+          <t>KCP</t>
         </is>
       </c>
       <c r="C7" s="3" t="n">
-        <v>2998.999843288399</v>
+        <v>241.4045174656262</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>2.325581395348837</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="8">
@@ -577,14 +577,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SCHAEFFLER</t>
+          <t>GODFRYPHLP</t>
         </is>
       </c>
       <c r="C8" s="3" t="n">
-        <v>4747.486630466043</v>
+        <v>10309.96754222702</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>2.325581395348837</v>
+        <v>4.444444444444445</v>
       </c>
     </row>
     <row r="9">
@@ -593,14 +593,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>UPL</t>
+          <t>NATIONALUM</t>
         </is>
       </c>
       <c r="C9" s="3" t="n">
-        <v>746.5463222727701</v>
+        <v>215.4321943982202</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>6.976744186046512</v>
+        <v>2.222222222222222</v>
       </c>
     </row>
     <row r="10">
@@ -609,14 +609,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CRAFTSMAN</t>
+          <t>ANGELONE</t>
         </is>
       </c>
       <c r="C10" s="3" t="n">
-        <v>7111.741741431812</v>
+        <v>2996.321922184466</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>2.325581395348837</v>
+        <v>4.444444444444445</v>
       </c>
     </row>
     <row r="11">
@@ -625,14 +625,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ASHAPURMIN</t>
+          <t>AGI</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>622.7105881821097</v>
+        <v>975.6139318380255</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>4.651162790697675</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="12">
@@ -641,14 +641,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CHEMPLASTS</t>
+          <t>BALKRISIND</t>
         </is>
       </c>
       <c r="C12" s="3" t="n">
-        <v>479.8745961253245</v>
+        <v>2996.566086235543</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>6.976744186046512</v>
+        <v>2.222222222222222</v>
       </c>
     </row>
     <row r="13">
@@ -657,14 +657,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>METROBRAND</t>
+          <t>MAPMYINDIA</t>
         </is>
       </c>
       <c r="C13" s="3" t="n">
-        <v>1300.862736668633</v>
+        <v>1956.352294224842</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>2.325581395348837</v>
+        <v>4.444444444444445</v>
       </c>
     </row>
     <row r="14">
@@ -673,14 +673,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SUNTV</t>
+          <t>RAMCOCEM</t>
         </is>
       </c>
       <c r="C14" s="3" t="n">
-        <v>634.4313398645224</v>
+        <v>1275.847933850921</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>2.325581395348837</v>
+        <v>2.222222222222222</v>
       </c>
     </row>
     <row r="15">
@@ -689,14 +689,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>POONAWALLA</t>
+          <t>SWIGGY</t>
         </is>
       </c>
       <c r="C15" s="3" t="n">
-        <v>490.3154832072964</v>
+        <v>425.8872986524872</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>2.325581395348837</v>
+        <v>8.888888888888889</v>
       </c>
     </row>
     <row r="16">
@@ -705,14 +705,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TATAINVEST</t>
+          <t>KEI</t>
         </is>
       </c>
       <c r="C16" s="3" t="n">
-        <v>7184.423831922282</v>
+        <v>4245.947657859202</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>4.651162790697675</v>
+        <v>2.222222222222222</v>
       </c>
     </row>
     <row r="17">
@@ -721,14 +721,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TIMKEN</t>
+          <t>GMDCLTD</t>
         </is>
       </c>
       <c r="C17" s="3" t="n">
-        <v>3561.631160176454</v>
+        <v>464.5531243299245</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>6.976744186046512</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="18">
@@ -737,14 +737,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PRAKASH</t>
+          <t>AMBUJACEM</t>
         </is>
       </c>
       <c r="C18" s="3" t="n">
-        <v>185.7201128938527</v>
+        <v>643.7458124196876</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>6.976744186046512</v>
+        <v>4.444444444444445</v>
       </c>
     </row>
     <row r="19">
@@ -753,14 +753,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>TATASTEEL</t>
+          <t>SAMMAANCAP</t>
         </is>
       </c>
       <c r="C19" s="3" t="n">
-        <v>168.7678033002403</v>
+        <v>145.6604801783684</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>4.651162790697675</v>
+        <v>2.222222222222222</v>
       </c>
     </row>
     <row r="20">
@@ -769,14 +769,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>FLUOROCHEM</t>
+          <t>EXIDEIND</t>
         </is>
       </c>
       <c r="C20" s="3" t="n">
-        <v>3653.500678453571</v>
+        <v>413.5690856132377</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>4.651162790697675</v>
+        <v>2.222222222222222</v>
       </c>
     </row>
     <row r="21">
@@ -785,14 +785,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>VBL</t>
+          <t>SUMICHEM</t>
         </is>
       </c>
       <c r="C21" s="3" t="n">
-        <v>499.5081586398466</v>
+        <v>621.1262396594908</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>4.651162790697675</v>
+        <v>2.222222222222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>